<commit_message>
Fix for Mac Excel
</commit_message>
<xml_diff>
--- a/output/file.xlsx
+++ b/output/file.xlsx
@@ -673,7 +673,7 @@
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="12192000" cy="1905000"/>
+    <xdr:ext cx="13458825" cy="1905000"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="1" name="Logo" descr="Logo">
@@ -705,7 +705,7 @@
       <xdr:row>12</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="5486400" cy="2457450"/>
+    <xdr:ext cx="6057900" cy="2457450"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="" descr=""/>

</xml_diff>